<commit_message>
caso de prueba ingles
</commit_message>
<xml_diff>
--- a/Diseños_test.xlsx
+++ b/Diseños_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRAN\Documents\Genially_Cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B589570-290E-4348-A7C7-0856AC906E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68793D37-5508-498F-B7AD-D475FC386917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="92">
   <si>
     <t>Titulo</t>
   </si>
@@ -81,193 +81,10 @@
     <t>Captura</t>
   </si>
   <si>
-    <t xml:space="preserve">Realiza login con datos incorrectos y posteriormente el correcto </t>
-  </si>
-  <si>
     <t>Navega a la web de Genially</t>
   </si>
   <si>
     <t>Navega correctamente a la web</t>
-  </si>
-  <si>
-    <t>Navega correctamente al portal de login</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Muestra la contraseña con formato válido</t>
-  </si>
-  <si>
-    <r>
-      <t>Selecciona el botón</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Acceder</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Selecciona el botón </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Entrar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Introducir contraseña correcta "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GN2021fran</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Introducir email con el formato sin @ "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <t>Muestra el email con el formato correcto</t>
-  </si>
-  <si>
-    <r>
-      <t>Introduce una contraseña incorrecta "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>123456</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Introducir email con el formato correcto "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>frantestingcy@yahoo.com</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
-    <t>Muestra la contraseña con formato inválido</t>
-  </si>
-  <si>
-    <r>
-      <t>Muestra el mensaje de error correctamente "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Email o contraseña incorrecto</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>".</t>
-    </r>
-  </si>
-  <si>
-    <t>Muestra el email con el formato incorrecto</t>
-  </si>
-  <si>
-    <t>Accede correctamente al portal del usuario</t>
   </si>
   <si>
     <t>2 - Planes</t>
@@ -990,6 +807,263 @@
       </rPr>
       <t>Registrate con tu email</t>
     </r>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>Operative System</t>
+  </si>
+  <si>
+    <t>Pre-conditions</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Unauthenticated user</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Visit the Genially web</t>
+  </si>
+  <si>
+    <t>Visit the Genially web correctly</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Press the button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enter the email format without @ "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Login with incorrect credentials and then with correct credentials</t>
+  </si>
+  <si>
+    <r>
+      <t>Enter the correct password "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GN2021fran</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Press the button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Log in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enter the email with the correct format  "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>frantestingcy@yahoo.com</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enter the incorrect password "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>123456</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enter the correct password  "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GN2021fran</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <r>
+      <t>Display the error message "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Incorrect email or password</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>".</t>
+    </r>
+  </si>
+  <si>
+    <t>Display the email with correct format</t>
+  </si>
+  <si>
+    <t>Navigate to the login portal</t>
+  </si>
+  <si>
+    <t>Display the email with the wrong format</t>
+  </si>
+  <si>
+    <t>Display the password in correct format</t>
+  </si>
+  <si>
+    <t>Display the password with the wrong format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access and check the user profile </t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1087,6 +1161,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,8 +1243,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3093758</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>2143125</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>933450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2590,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,13 +2681,13 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
@@ -2618,13 +2695,13 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>9</v>
@@ -2632,40 +2709,40 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+        <v>69</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2673,10 +2750,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -2685,10 +2762,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>76</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2697,10 +2774,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
+        <v>77</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -2709,22 +2786,22 @@
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>79</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:5" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -2733,10 +2810,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>26</v>
+        <v>81</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E12" s="4"/>
     </row>
@@ -2745,10 +2822,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>82</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="E13" s="4"/>
     </row>
@@ -2756,11 +2833,11 @@
       <c r="B14" s="3">
         <v>8</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>30</v>
+      <c r="C14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -2769,10 +2846,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>26</v>
+        <v>81</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E15" s="4"/>
     </row>
@@ -2781,10 +2858,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
+        <v>83</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="E16" s="4"/>
     </row>
@@ -2792,11 +2869,11 @@
       <c r="B17" s="3">
         <v>11</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>32</v>
+      <c r="C17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -2831,7 +2908,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -2872,11 +2949,11 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -2897,10 +2974,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -2909,10 +2986,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2921,10 +2998,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -2933,10 +3010,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -2954,7 +3031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7793A5-AC40-4E61-98B2-281DD4AFC0FC}">
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
@@ -2971,7 +3048,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -2999,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -3012,11 +3089,11 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -3037,10 +3114,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -3049,10 +3126,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -3061,10 +3138,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -3073,10 +3150,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -3085,10 +3162,10 @@
         <v>5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -3097,10 +3174,10 @@
         <v>6</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E12" s="6"/>
     </row>
@@ -3109,10 +3186,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -3121,10 +3198,10 @@
         <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -3133,10 +3210,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E15" s="6"/>
     </row>
@@ -3145,10 +3222,10 @@
         <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -3166,7 +3243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7101634C-BD7B-4144-BB41-202E6A63C934}">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3183,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -3217,18 +3294,18 @@
         <v>5</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
@@ -3249,10 +3326,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -3261,10 +3338,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -3273,10 +3350,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -3285,10 +3362,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -3297,10 +3374,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -3309,10 +3386,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -3321,10 +3398,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -3333,10 +3410,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -3345,10 +3422,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1"/>
     </row>

</xml_diff>